<commit_message>
fixed monte carlo for ties
</commit_message>
<xml_diff>
--- a/leagues/0755 Fantasy Football 2025.xlsx
+++ b/leagues/0755 Fantasy Football 2025.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="89">
   <si>
     <t>Michael, The Baker</t>
   </si>
@@ -149,31 +149,37 @@
     <t>1-3</t>
   </si>
   <si>
-    <t>9.3-4.7</t>
-  </si>
-  <si>
-    <t>8.6-5.4</t>
-  </si>
-  <si>
-    <t>7.9-6.1</t>
-  </si>
-  <si>
-    <t>7.3-6.7</t>
-  </si>
-  <si>
-    <t>7.0-7.0</t>
-  </si>
-  <si>
-    <t>6.9-7.1</t>
-  </si>
-  <si>
-    <t>6.4-7.6</t>
-  </si>
-  <si>
-    <t>5.3-8.7</t>
-  </si>
-  <si>
-    <t>4.8-9.2</t>
+    <t>9.3-4.7-0.1</t>
+  </si>
+  <si>
+    <t>8.5-5.4-0.1</t>
+  </si>
+  <si>
+    <t>7.9-6.1-0.1</t>
+  </si>
+  <si>
+    <t>7.2-6.8</t>
+  </si>
+  <si>
+    <t>7.0-7.0-0.1</t>
+  </si>
+  <si>
+    <t>6.8-7.1-0.1</t>
+  </si>
+  <si>
+    <t>6.4-7.5-0.1</t>
+  </si>
+  <si>
+    <t>6.5-7.4-0.1</t>
+  </si>
+  <si>
+    <t>5.3-8.6-0.1</t>
+  </si>
+  <si>
+    <t>4.8-9.2-0.1</t>
+  </si>
+  <si>
+    <t>10-4</t>
   </si>
   <si>
     <t>9-5</t>
@@ -183,9 +189,6 @@
   </si>
   <si>
     <t>7-7</t>
-  </si>
-  <si>
-    <t>6-8</t>
   </si>
   <si>
     <t>5-9</t>
@@ -1447,37 +1450,37 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>47.7</v>
+        <v>47.2</v>
       </c>
       <c r="C2">
-        <v>22.6</v>
+        <v>23.1</v>
       </c>
       <c r="D2">
-        <v>12.8</v>
+        <v>11.9</v>
       </c>
       <c r="E2">
-        <v>7.7</v>
+        <v>8.1</v>
       </c>
       <c r="F2">
-        <v>3.9</v>
+        <v>3.7</v>
       </c>
       <c r="G2">
-        <v>3.1</v>
+        <v>3.4</v>
       </c>
       <c r="H2">
-        <v>1.2</v>
+        <v>1.3</v>
       </c>
       <c r="I2">
-        <v>0.7</v>
+        <v>0.9</v>
       </c>
       <c r="J2">
         <v>0.3</v>
       </c>
       <c r="K2">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="L2">
-        <v>97.8</v>
+        <v>97.40000000000001</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -1485,37 +1488,37 @@
         <v>8</v>
       </c>
       <c r="B3">
-        <v>21.1</v>
+        <v>23.3</v>
       </c>
       <c r="C3">
-        <v>25.1</v>
+        <v>22.3</v>
       </c>
       <c r="D3">
-        <v>19.4</v>
+        <v>16.1</v>
       </c>
       <c r="E3">
-        <v>9.300000000000001</v>
+        <v>13.4</v>
       </c>
       <c r="F3">
-        <v>10.6</v>
+        <v>8.5</v>
       </c>
       <c r="G3">
-        <v>6.1</v>
+        <v>6.7</v>
       </c>
       <c r="H3">
-        <v>3.7</v>
+        <v>4.4</v>
       </c>
       <c r="I3">
-        <v>2.5</v>
+        <v>2.7</v>
       </c>
       <c r="J3">
-        <v>1.7</v>
+        <v>2</v>
       </c>
       <c r="K3">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
       <c r="L3">
-        <v>91.59999999999999</v>
+        <v>90.3</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -1523,37 +1526,37 @@
         <v>1</v>
       </c>
       <c r="B4">
+        <v>8.6</v>
+      </c>
+      <c r="C4">
+        <v>15.8</v>
+      </c>
+      <c r="D4">
+        <v>18.2</v>
+      </c>
+      <c r="E4">
+        <v>13.2</v>
+      </c>
+      <c r="F4">
+        <v>13.2</v>
+      </c>
+      <c r="G4">
         <v>11.2</v>
       </c>
-      <c r="C4">
-        <v>13.3</v>
-      </c>
-      <c r="D4">
-        <v>15.5</v>
-      </c>
-      <c r="E4">
-        <v>16.4</v>
-      </c>
-      <c r="F4">
-        <v>12.5</v>
-      </c>
-      <c r="G4">
-        <v>9.1</v>
-      </c>
       <c r="H4">
-        <v>8.699999999999999</v>
+        <v>7.9</v>
       </c>
       <c r="I4">
-        <v>7.7</v>
+        <v>7</v>
       </c>
       <c r="J4">
-        <v>3.5</v>
+        <v>4.1</v>
       </c>
       <c r="K4">
-        <v>2.1</v>
+        <v>0.8</v>
       </c>
       <c r="L4">
-        <v>78</v>
+        <v>80.2</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -1561,37 +1564,37 @@
         <v>6</v>
       </c>
       <c r="B5">
-        <v>7.8</v>
+        <v>7.2</v>
       </c>
       <c r="C5">
-        <v>11.3</v>
+        <v>11.4</v>
       </c>
       <c r="D5">
         <v>13.3</v>
       </c>
       <c r="E5">
-        <v>14.6</v>
+        <v>12.2</v>
       </c>
       <c r="F5">
-        <v>13.6</v>
+        <v>14.4</v>
       </c>
       <c r="G5">
-        <v>12.7</v>
+        <v>13.3</v>
       </c>
       <c r="H5">
-        <v>9.4</v>
+        <v>10.2</v>
       </c>
       <c r="I5">
-        <v>8.1</v>
+        <v>8.300000000000001</v>
       </c>
       <c r="J5">
-        <v>6.3</v>
+        <v>6</v>
       </c>
       <c r="K5">
-        <v>2.9</v>
+        <v>3.7</v>
       </c>
       <c r="L5">
-        <v>73.3</v>
+        <v>71.8</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -1599,37 +1602,37 @@
         <v>2</v>
       </c>
       <c r="B6">
-        <v>4</v>
+        <v>4.1</v>
       </c>
       <c r="C6">
-        <v>9.199999999999999</v>
+        <v>8.9</v>
       </c>
       <c r="D6">
-        <v>11.3</v>
+        <v>12.3</v>
       </c>
       <c r="E6">
-        <v>12.4</v>
+        <v>11.8</v>
       </c>
       <c r="F6">
-        <v>14.7</v>
+        <v>11.8</v>
       </c>
       <c r="G6">
-        <v>14.2</v>
+        <v>14.1</v>
       </c>
       <c r="H6">
-        <v>12.1</v>
+        <v>12.5</v>
       </c>
       <c r="I6">
-        <v>10.6</v>
+        <v>11.5</v>
       </c>
       <c r="J6">
-        <v>8.300000000000001</v>
+        <v>8.4</v>
       </c>
       <c r="K6">
-        <v>3.2</v>
+        <v>4.6</v>
       </c>
       <c r="L6">
-        <v>65.8</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -1637,37 +1640,37 @@
         <v>9</v>
       </c>
       <c r="B7">
-        <v>3.6</v>
+        <v>3.8</v>
       </c>
       <c r="C7">
-        <v>6.5</v>
+        <v>6.4</v>
       </c>
       <c r="D7">
-        <v>11</v>
+        <v>9.4</v>
       </c>
       <c r="E7">
-        <v>12.8</v>
+        <v>13.6</v>
       </c>
       <c r="F7">
-        <v>12.4</v>
+        <v>11.8</v>
       </c>
       <c r="G7">
-        <v>13.2</v>
+        <v>12.6</v>
       </c>
       <c r="H7">
-        <v>14.5</v>
+        <v>13.4</v>
       </c>
       <c r="I7">
-        <v>11.7</v>
+        <v>13</v>
       </c>
       <c r="J7">
-        <v>9.699999999999999</v>
+        <v>10.2</v>
       </c>
       <c r="K7">
-        <v>4.6</v>
+        <v>5.8</v>
       </c>
       <c r="L7">
-        <v>59.5</v>
+        <v>57.6</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -1675,37 +1678,37 @@
         <v>5</v>
       </c>
       <c r="B8">
-        <v>2.7</v>
+        <v>3.9</v>
       </c>
       <c r="C8">
-        <v>7</v>
+        <v>6.9</v>
       </c>
       <c r="D8">
-        <v>8.5</v>
+        <v>8.800000000000001</v>
       </c>
       <c r="E8">
+        <v>11.6</v>
+      </c>
+      <c r="F8">
+        <v>13.1</v>
+      </c>
+      <c r="G8">
+        <v>11.3</v>
+      </c>
+      <c r="H8">
+        <v>14.4</v>
+      </c>
+      <c r="I8">
         <v>11.2</v>
       </c>
-      <c r="F8">
-        <v>13.6</v>
-      </c>
-      <c r="G8">
-        <v>13</v>
-      </c>
-      <c r="H8">
-        <v>13.3</v>
-      </c>
-      <c r="I8">
-        <v>12.7</v>
-      </c>
       <c r="J8">
-        <v>11.5</v>
+        <v>11.2</v>
       </c>
       <c r="K8">
-        <v>6.5</v>
+        <v>7.6</v>
       </c>
       <c r="L8">
-        <v>56</v>
+        <v>55.6</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -1713,37 +1716,37 @@
         <v>4</v>
       </c>
       <c r="B9">
-        <v>1.2</v>
+        <v>1.8</v>
       </c>
       <c r="C9">
-        <v>3.2</v>
+        <v>3.8</v>
       </c>
       <c r="D9">
-        <v>5.3</v>
+        <v>7.1</v>
       </c>
       <c r="E9">
-        <v>10.2</v>
+        <v>10</v>
       </c>
       <c r="F9">
-        <v>12</v>
+        <v>13.6</v>
       </c>
       <c r="G9">
-        <v>14.9</v>
+        <v>14</v>
       </c>
       <c r="H9">
-        <v>17.7</v>
+        <v>16.5</v>
       </c>
       <c r="I9">
-        <v>16.1</v>
+        <v>15.1</v>
       </c>
       <c r="J9">
-        <v>13.7</v>
+        <v>11.6</v>
       </c>
       <c r="K9">
-        <v>5.7</v>
+        <v>6.5</v>
       </c>
       <c r="L9">
-        <v>46.8</v>
+        <v>50.3</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -1751,37 +1754,37 @@
         <v>3</v>
       </c>
       <c r="B10">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="C10">
-        <v>1.4</v>
+        <v>0.9</v>
       </c>
       <c r="D10">
-        <v>2.1</v>
+        <v>1.8</v>
       </c>
       <c r="E10">
-        <v>3.4</v>
+        <v>4.1</v>
       </c>
       <c r="F10">
-        <v>4.5</v>
+        <v>6.2</v>
       </c>
       <c r="G10">
-        <v>8.6</v>
+        <v>9.4</v>
       </c>
       <c r="H10">
-        <v>11.7</v>
+        <v>11.2</v>
       </c>
       <c r="I10">
-        <v>17.3</v>
+        <v>17.4</v>
       </c>
       <c r="J10">
-        <v>24.1</v>
+        <v>25.1</v>
       </c>
       <c r="K10">
-        <v>26.4</v>
+        <v>23.9</v>
       </c>
       <c r="L10">
-        <v>20.5</v>
+        <v>22.4</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -1789,37 +1792,37 @@
         <v>7</v>
       </c>
       <c r="B11">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="C11">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="D11">
-        <v>0.8</v>
+        <v>1.1</v>
       </c>
       <c r="E11">
         <v>2</v>
       </c>
       <c r="F11">
-        <v>2.2</v>
+        <v>3.7</v>
       </c>
       <c r="G11">
-        <v>5.1</v>
+        <v>4</v>
       </c>
       <c r="H11">
-        <v>7.7</v>
+        <v>8.199999999999999</v>
       </c>
       <c r="I11">
-        <v>12.6</v>
+        <v>12.9</v>
       </c>
       <c r="J11">
-        <v>20.9</v>
+        <v>21.1</v>
       </c>
       <c r="K11">
-        <v>48.1</v>
+        <v>46.4</v>
       </c>
       <c r="L11">
-        <v>10.7</v>
+        <v>11.4</v>
       </c>
     </row>
   </sheetData>
@@ -1878,13 +1881,13 @@
         <v>549.9200000000001</v>
       </c>
       <c r="F2">
-        <v>97.8</v>
+        <v>97.39999999999999</v>
       </c>
       <c r="G2" t="s">
         <v>42</v>
       </c>
       <c r="H2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -1904,13 +1907,13 @@
         <v>499.16</v>
       </c>
       <c r="F3">
-        <v>91.60000000000001</v>
+        <v>90.3</v>
       </c>
       <c r="G3" t="s">
         <v>43</v>
       </c>
       <c r="H3" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -1930,13 +1933,13 @@
         <v>466.16</v>
       </c>
       <c r="F4">
-        <v>78</v>
+        <v>80.2</v>
       </c>
       <c r="G4" t="s">
         <v>44</v>
       </c>
       <c r="H4" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -1956,13 +1959,13 @@
         <v>494.06</v>
       </c>
       <c r="F5">
-        <v>73.3</v>
+        <v>71.8</v>
       </c>
       <c r="G5" t="s">
         <v>45</v>
       </c>
       <c r="H5" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -1982,13 +1985,13 @@
         <v>473.2</v>
       </c>
       <c r="F6">
-        <v>65.8</v>
+        <v>63</v>
       </c>
       <c r="G6" t="s">
         <v>46</v>
       </c>
       <c r="H6" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -2008,13 +2011,13 @@
         <v>464.46</v>
       </c>
       <c r="F7">
-        <v>59.5</v>
+        <v>57.59999999999999</v>
       </c>
       <c r="G7" t="s">
         <v>47</v>
       </c>
       <c r="H7" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -2034,13 +2037,13 @@
         <v>499.16</v>
       </c>
       <c r="F8">
-        <v>56.00000000000001</v>
+        <v>55.60000000000001</v>
       </c>
       <c r="G8" t="s">
         <v>48</v>
       </c>
       <c r="H8" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -2060,13 +2063,13 @@
         <v>454.66</v>
       </c>
       <c r="F9">
-        <v>46.8</v>
+        <v>50.3</v>
       </c>
       <c r="G9" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H9" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -2086,13 +2089,13 @@
         <v>435.1800000000001</v>
       </c>
       <c r="F10">
-        <v>20.5</v>
+        <v>22.4</v>
       </c>
       <c r="G10" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H10" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -2112,13 +2115,13 @@
         <v>398.86</v>
       </c>
       <c r="F11">
-        <v>10.7</v>
+        <v>11.4</v>
       </c>
       <c r="G11" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="H11" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -2139,16 +2142,16 @@
         <v>15</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>17</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -2159,7 +2162,7 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D2">
         <v>11</v>
@@ -2168,7 +2171,7 @@
         <v>10</v>
       </c>
       <c r="F2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -2179,7 +2182,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D3">
         <v>10</v>
@@ -2188,7 +2191,7 @@
         <v>11</v>
       </c>
       <c r="F3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -2199,7 +2202,7 @@
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D4">
         <v>6</v>
@@ -2208,7 +2211,7 @@
         <v>12</v>
       </c>
       <c r="F4" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -2219,7 +2222,7 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D5">
         <v>2</v>
@@ -2228,7 +2231,7 @@
         <v>12</v>
       </c>
       <c r="F5" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -2239,7 +2242,7 @@
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -2248,7 +2251,7 @@
         <v>11</v>
       </c>
       <c r="F6" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -2259,7 +2262,7 @@
         <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D7">
         <v>-1</v>
@@ -2268,7 +2271,7 @@
         <v>10</v>
       </c>
       <c r="F7" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -2279,7 +2282,7 @@
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D8">
         <v>-1</v>
@@ -2288,7 +2291,7 @@
         <v>10</v>
       </c>
       <c r="F8" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -2299,7 +2302,7 @@
         <v>4</v>
       </c>
       <c r="C9" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D9">
         <v>-4</v>
@@ -2308,7 +2311,7 @@
         <v>11</v>
       </c>
       <c r="F9" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -2319,7 +2322,7 @@
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D10">
         <v>-10</v>
@@ -2328,7 +2331,7 @@
         <v>11</v>
       </c>
       <c r="F10" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -2339,7 +2342,7 @@
         <v>7</v>
       </c>
       <c r="C11" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D11">
         <v>-13</v>
@@ -2348,7 +2351,7 @@
         <v>12</v>
       </c>
       <c r="F11" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -2366,19 +2369,19 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="B1" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -2398,7 +2401,7 @@
         <v>11</v>
       </c>
       <c r="F2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -2418,7 +2421,7 @@
         <v>10</v>
       </c>
       <c r="F3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -2438,7 +2441,7 @@
         <v>6</v>
       </c>
       <c r="F4" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -2458,7 +2461,7 @@
         <v>2</v>
       </c>
       <c r="F5" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -2478,7 +2481,7 @@
         <v>0</v>
       </c>
       <c r="F6" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -2498,7 +2501,7 @@
         <v>-1</v>
       </c>
       <c r="F7" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -2518,7 +2521,7 @@
         <v>-1</v>
       </c>
       <c r="F8" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -2538,7 +2541,7 @@
         <v>-4</v>
       </c>
       <c r="F9" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -2558,7 +2561,7 @@
         <v>-10</v>
       </c>
       <c r="F10" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -2578,7 +2581,7 @@
         <v>-13</v>
       </c>
       <c r="F11" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -2596,25 +2599,25 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="B1" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:8">

</xml_diff>